<commit_message>
chore: add nearest neighbour to scatter and tabu
</commit_message>
<xml_diff>
--- a/assets/results/tabu_results.xlsx
+++ b/assets/results/tabu_results.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,118 +413,711 @@
         <v>Result Cost</v>
       </c>
       <c r="D1" t="str">
+        <v>Initial Cost (Nearest Neighbor)</v>
+      </c>
+      <c r="E1" t="str">
         <v>Time</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Deviation</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Parameters</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>kroA100</v>
+        <v>a280</v>
       </c>
       <c r="B2">
-        <v>21282</v>
+        <v>2579</v>
       </c>
       <c r="C2">
-        <v>22171</v>
-      </c>
-      <c r="D2" t="str">
-        <v>5.4s</v>
+        <v>2698</v>
+      </c>
+      <c r="D2">
+        <v>3450</v>
       </c>
       <c r="E2" t="str">
-        <v>4.18%</v>
+        <v>20.3s</v>
       </c>
       <c r="F2" t="str">
-        <v>[500]</v>
+        <v>4.60%</v>
+      </c>
+      <c r="G2" t="str">
+        <v>[100]</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>kroA150</v>
+        <v>bier127</v>
       </c>
       <c r="B3">
-        <v>26524</v>
+        <v>118282</v>
       </c>
       <c r="C3">
-        <v>27371</v>
-      </c>
-      <c r="D3" t="str">
-        <v>20.1s</v>
+        <v>121342</v>
+      </c>
+      <c r="D3">
+        <v>141504</v>
       </c>
       <c r="E3" t="str">
-        <v>3.20%</v>
+        <v>1.9s</v>
       </c>
       <c r="F3" t="str">
-        <v>[500]</v>
+        <v>2.59%</v>
+      </c>
+      <c r="G3" t="str">
+        <v>[100]</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>kroA200</v>
+        <v>ch130</v>
       </c>
       <c r="B4">
-        <v>29368</v>
+        <v>6110</v>
       </c>
       <c r="C4">
-        <v>30497</v>
-      </c>
-      <c r="D4" t="str">
-        <v>46.3s</v>
+        <v>6427</v>
+      </c>
+      <c r="D4">
+        <v>7673</v>
       </c>
       <c r="E4" t="str">
-        <v>3.85%</v>
+        <v>2.8s</v>
       </c>
       <c r="F4" t="str">
-        <v>[500]</v>
+        <v>5.18%</v>
+      </c>
+      <c r="G4" t="str">
+        <v>[100]</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>kroB100</v>
+        <v>ch150</v>
       </c>
       <c r="B5">
-        <v>22141</v>
+        <v>6528</v>
       </c>
       <c r="C5">
-        <v>22949</v>
-      </c>
-      <c r="D5" t="str">
-        <v>5.9s</v>
+        <v>6595</v>
+      </c>
+      <c r="D5">
+        <v>8317</v>
       </c>
       <c r="E5" t="str">
-        <v>3.65%</v>
+        <v>4.2s</v>
       </c>
       <c r="F5" t="str">
-        <v>[500]</v>
+        <v>1.03%</v>
+      </c>
+      <c r="G5" t="str">
+        <v>[100]</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>d198</v>
+      </c>
+      <c r="B6">
+        <v>15780</v>
+      </c>
+      <c r="C6">
+        <v>16070</v>
+      </c>
+      <c r="D6">
+        <v>17979</v>
+      </c>
+      <c r="E6" t="str">
+        <v>9.2s</v>
+      </c>
+      <c r="F6" t="str">
+        <v>1.84%</v>
+      </c>
+      <c r="G6" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>eil101</v>
+      </c>
+      <c r="B7">
+        <v>629</v>
+      </c>
+      <c r="C7">
+        <v>646</v>
+      </c>
+      <c r="D7">
+        <v>780</v>
+      </c>
+      <c r="E7" t="str">
+        <v>1.1s</v>
+      </c>
+      <c r="F7" t="str">
+        <v>2.70%</v>
+      </c>
+      <c r="G7" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>gil262</v>
+      </c>
+      <c r="B8">
+        <v>2378</v>
+      </c>
+      <c r="C8">
+        <v>2481</v>
+      </c>
+      <c r="D8">
+        <v>3170</v>
+      </c>
+      <c r="E8" t="str">
+        <v>19.1s</v>
+      </c>
+      <c r="F8" t="str">
+        <v>4.33%</v>
+      </c>
+      <c r="G8" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>kroA100</v>
+      </c>
+      <c r="B9">
+        <v>21282</v>
+      </c>
+      <c r="C9">
+        <v>21395</v>
+      </c>
+      <c r="D9">
+        <v>26470</v>
+      </c>
+      <c r="E9" t="str">
+        <v>1.0s</v>
+      </c>
+      <c r="F9" t="str">
+        <v>0.53%</v>
+      </c>
+      <c r="G9" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>kroA150</v>
+      </c>
+      <c r="B10">
+        <v>26524</v>
+      </c>
+      <c r="C10">
+        <v>27873</v>
+      </c>
+      <c r="D10">
+        <v>33744</v>
+      </c>
+      <c r="E10" t="str">
+        <v>3.5s</v>
+      </c>
+      <c r="F10" t="str">
+        <v>5.09%</v>
+      </c>
+      <c r="G10" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>kroA200</v>
+      </c>
+      <c r="B11">
+        <v>29368</v>
+      </c>
+      <c r="C11">
+        <v>31089</v>
+      </c>
+      <c r="D11">
+        <v>41544</v>
+      </c>
+      <c r="E11" t="str">
+        <v>8.7s</v>
+      </c>
+      <c r="F11" t="str">
+        <v>5.86%</v>
+      </c>
+      <c r="G11" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>kroB100</v>
+      </c>
+      <c r="B12">
+        <v>22141</v>
+      </c>
+      <c r="C12">
+        <v>22354</v>
+      </c>
+      <c r="D12">
+        <v>28579</v>
+      </c>
+      <c r="E12" t="str">
+        <v>1.1s</v>
+      </c>
+      <c r="F12" t="str">
+        <v>0.96%</v>
+      </c>
+      <c r="G12" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
         <v>kroB150</v>
       </c>
-      <c r="B6">
+      <c r="B13">
         <v>26130</v>
       </c>
-      <c r="C6">
-        <v>26617</v>
-      </c>
-      <c r="D6" t="str">
-        <v>19.1s</v>
-      </c>
-      <c r="E6" t="str">
+      <c r="C13">
+        <v>26791</v>
+      </c>
+      <c r="D13">
+        <v>35334</v>
+      </c>
+      <c r="E13" t="str">
+        <v>3.8s</v>
+      </c>
+      <c r="F13" t="str">
+        <v>2.53%</v>
+      </c>
+      <c r="G13" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>kroB200</v>
+      </c>
+      <c r="B14">
+        <v>29437</v>
+      </c>
+      <c r="C14">
+        <v>30995</v>
+      </c>
+      <c r="D14">
+        <v>36757</v>
+      </c>
+      <c r="E14" t="str">
+        <v>7.9s</v>
+      </c>
+      <c r="F14" t="str">
+        <v>5.29%</v>
+      </c>
+      <c r="G14" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>kroC100</v>
+      </c>
+      <c r="B15">
+        <v>20749</v>
+      </c>
+      <c r="C15">
+        <v>21500</v>
+      </c>
+      <c r="D15">
+        <v>24955</v>
+      </c>
+      <c r="E15" t="str">
+        <v>0.9s</v>
+      </c>
+      <c r="F15" t="str">
+        <v>3.62%</v>
+      </c>
+      <c r="G15" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>kroD100</v>
+      </c>
+      <c r="B16">
+        <v>21294</v>
+      </c>
+      <c r="C16">
+        <v>21708</v>
+      </c>
+      <c r="D16">
+        <v>27734</v>
+      </c>
+      <c r="E16" t="str">
+        <v>0.9s</v>
+      </c>
+      <c r="F16" t="str">
+        <v>1.94%</v>
+      </c>
+      <c r="G16" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>kroE100</v>
+      </c>
+      <c r="B17">
+        <v>22068</v>
+      </c>
+      <c r="C17">
+        <v>22759</v>
+      </c>
+      <c r="D17">
+        <v>28674</v>
+      </c>
+      <c r="E17" t="str">
+        <v>0.9s</v>
+      </c>
+      <c r="F17" t="str">
+        <v>3.13%</v>
+      </c>
+      <c r="G17" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>lin105</v>
+      </c>
+      <c r="B18">
+        <v>14379</v>
+      </c>
+      <c r="C18">
+        <v>14646</v>
+      </c>
+      <c r="D18">
+        <v>18216</v>
+      </c>
+      <c r="E18" t="str">
+        <v>1.0s</v>
+      </c>
+      <c r="F18" t="str">
         <v>1.86%</v>
       </c>
-      <c r="F6" t="str">
-        <v>[500]</v>
+      <c r="G18" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>pr107</v>
+      </c>
+      <c r="B19">
+        <v>44303</v>
+      </c>
+      <c r="C19">
+        <v>44497</v>
+      </c>
+      <c r="D19">
+        <v>51913</v>
+      </c>
+      <c r="E19" t="str">
+        <v>1.1s</v>
+      </c>
+      <c r="F19" t="str">
+        <v>0.44%</v>
+      </c>
+      <c r="G19" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>pr124</v>
+      </c>
+      <c r="B20">
+        <v>59030</v>
+      </c>
+      <c r="C20">
+        <v>59795</v>
+      </c>
+      <c r="D20">
+        <v>67304</v>
+      </c>
+      <c r="E20" t="str">
+        <v>1.7s</v>
+      </c>
+      <c r="F20" t="str">
+        <v>1.30%</v>
+      </c>
+      <c r="G20" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>pr136</v>
+      </c>
+      <c r="B21">
+        <v>96772</v>
+      </c>
+      <c r="C21">
+        <v>102981</v>
+      </c>
+      <c r="D21">
+        <v>120813</v>
+      </c>
+      <c r="E21" t="str">
+        <v>2.3s</v>
+      </c>
+      <c r="F21" t="str">
+        <v>6.42%</v>
+      </c>
+      <c r="G21" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>pr144</v>
+      </c>
+      <c r="B22">
+        <v>58537</v>
+      </c>
+      <c r="C22">
+        <v>58761</v>
+      </c>
+      <c r="D22">
+        <v>70784</v>
+      </c>
+      <c r="E22" t="str">
+        <v>2.7s</v>
+      </c>
+      <c r="F22" t="str">
+        <v>0.38%</v>
+      </c>
+      <c r="G22" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>pr152</v>
+      </c>
+      <c r="B23">
+        <v>73682</v>
+      </c>
+      <c r="C23">
+        <v>74426</v>
+      </c>
+      <c r="D23">
+        <v>94727</v>
+      </c>
+      <c r="E23" t="str">
+        <v>3.3s</v>
+      </c>
+      <c r="F23" t="str">
+        <v>1.01%</v>
+      </c>
+      <c r="G23" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>pr226</v>
+      </c>
+      <c r="B24">
+        <v>80369</v>
+      </c>
+      <c r="C24">
+        <v>83983</v>
+      </c>
+      <c r="D24">
+        <v>93859</v>
+      </c>
+      <c r="E24" t="str">
+        <v>10.6s</v>
+      </c>
+      <c r="F24" t="str">
+        <v>4.50%</v>
+      </c>
+      <c r="G24" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>pr264</v>
+      </c>
+      <c r="B25">
+        <v>49135</v>
+      </c>
+      <c r="C25">
+        <v>51302</v>
+      </c>
+      <c r="D25">
+        <v>58324</v>
+      </c>
+      <c r="E25" t="str">
+        <v>16.8s</v>
+      </c>
+      <c r="F25" t="str">
+        <v>4.41%</v>
+      </c>
+      <c r="G25" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>pr299</v>
+      </c>
+      <c r="B26">
+        <v>48191</v>
+      </c>
+      <c r="C26">
+        <v>50380</v>
+      </c>
+      <c r="D26">
+        <v>67024</v>
+      </c>
+      <c r="E26" t="str">
+        <v>24.3s</v>
+      </c>
+      <c r="F26" t="str">
+        <v>4.54%</v>
+      </c>
+      <c r="G26" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>rat195</v>
+      </c>
+      <c r="B27">
+        <v>2323</v>
+      </c>
+      <c r="C27">
+        <v>2366</v>
+      </c>
+      <c r="D27">
+        <v>2643</v>
+      </c>
+      <c r="E27" t="str">
+        <v>6.8s</v>
+      </c>
+      <c r="F27" t="str">
+        <v>1.86%</v>
+      </c>
+      <c r="G27" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>rd100</v>
+      </c>
+      <c r="B28">
+        <v>7910</v>
+      </c>
+      <c r="C28">
+        <v>8197</v>
+      </c>
+      <c r="D28">
+        <v>9893</v>
+      </c>
+      <c r="E28" t="str">
+        <v>1.1s</v>
+      </c>
+      <c r="F28" t="str">
+        <v>3.63%</v>
+      </c>
+      <c r="G28" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>ts225</v>
+      </c>
+      <c r="B29">
+        <v>126643</v>
+      </c>
+      <c r="C29">
+        <v>134459</v>
+      </c>
+      <c r="D29">
+        <v>151438</v>
+      </c>
+      <c r="E29" t="str">
+        <v>10.9s</v>
+      </c>
+      <c r="F29" t="str">
+        <v>6.17%</v>
+      </c>
+      <c r="G29" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>tsp225</v>
+      </c>
+      <c r="B30">
+        <v>3916</v>
+      </c>
+      <c r="C30">
+        <v>3979</v>
+      </c>
+      <c r="D30">
+        <v>4972</v>
+      </c>
+      <c r="E30" t="str">
+        <v>11.5s</v>
+      </c>
+      <c r="F30" t="str">
+        <v>1.61%</v>
+      </c>
+      <c r="G30" t="str">
+        <v>[100]</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>u159</v>
+      </c>
+      <c r="B31">
+        <v>42080</v>
+      </c>
+      <c r="C31">
+        <v>46246</v>
+      </c>
+      <c r="D31">
+        <v>54942</v>
+      </c>
+      <c r="E31" t="str">
+        <v>3.7s</v>
+      </c>
+      <c r="F31" t="str">
+        <v>9.90%</v>
+      </c>
+      <c r="G31" t="str">
+        <v>[100]</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>